<commit_message>
Fin cours IA- Découverte base de données
</commit_message>
<xml_diff>
--- a/Seconde/2-03.xlsx
+++ b/Seconde/2-03.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lycée\Seconde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EBA4D9-84AE-4CB2-9533-DC86E086789A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22318807-7623-4146-B940-5732248D7713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E61A21D0-7BED-4373-9982-F4856F8C3D3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E61A21D0-7BED-4373-9982-F4856F8C3D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Groupe1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="63">
   <si>
     <t>Eval Blanche Lewis</t>
   </si>
@@ -208,20 +208,39 @@
     <t>Envoyé par paul</t>
   </si>
   <si>
-    <t>VidéoSNT</t>
-  </si>
-  <si>
     <t>Fait</t>
+  </si>
+  <si>
+    <t>RenduIntermSNT</t>
+  </si>
+  <si>
+    <t>VidéoEval</t>
+  </si>
+  <si>
+    <t>Note SNT intermediaire /4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,13 +284,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C7542E-EFA5-4F51-876B-29131A83BB32}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,14 +617,14 @@
     <col min="1" max="1" width="26.1796875" customWidth="1"/>
     <col min="2" max="3" width="2.6328125" customWidth="1"/>
     <col min="4" max="4" width="3.453125" customWidth="1"/>
-    <col min="5" max="5" width="5.7265625" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" customWidth="1"/>
+    <col min="5" max="5" width="2.54296875" customWidth="1"/>
+    <col min="6" max="6" width="1.6328125" customWidth="1"/>
     <col min="7" max="7" width="24.54296875" customWidth="1"/>
     <col min="8" max="8" width="21.7265625" customWidth="1"/>
     <col min="9" max="9" width="25.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -621,10 +641,13 @@
         <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -635,8 +658,12 @@
       <c r="F2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="4"/>
+      <c r="I2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -656,10 +683,14 @@
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -667,8 +698,9 @@
         <v>43</v>
       </c>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -681,8 +713,15 @@
       <c r="E5" s="5">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -696,8 +735,12 @@
         <v>43</v>
       </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -713,8 +756,12 @@
       <c r="F7" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="4"/>
+      <c r="I7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -725,8 +772,9 @@
         <v>43</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -743,10 +791,11 @@
         <v>0.75</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -766,10 +815,14 @@
         <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -779,8 +832,12 @@
       <c r="E11" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="4"/>
+      <c r="I11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -794,10 +851,14 @@
         <v>0.62</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -807,8 +868,15 @@
       <c r="E13" s="5">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -825,8 +893,15 @@
       <c r="F14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -843,10 +918,14 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -860,10 +939,14 @@
         <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -883,10 +966,14 @@
         <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -903,10 +990,14 @@
         <v>0.87</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -914,29 +1005,37 @@
         <v>46</v>
       </c>
       <c r="E19" s="1"/>
+      <c r="H19" s="4"/>
+      <c r="I19">
+        <v>3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D474A70D-55EF-4915-ABCA-C4E36266A098}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.81640625" customWidth="1"/>
     <col min="2" max="2" width="7.08984375" customWidth="1"/>
-    <col min="3" max="3" width="4.08984375" customWidth="1"/>
-    <col min="4" max="4" width="7.36328125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="15.36328125" customWidth="1"/>
+    <col min="7" max="7" width="27.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>38</v>
       </c>
@@ -946,8 +1045,17 @@
       <c r="D1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -955,10 +1063,14 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -969,10 +1081,14 @@
         <v>0.85</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -980,10 +1096,14 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -991,8 +1111,12 @@
       <c r="D5" s="5">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="4"/>
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1004,19 +1128,33 @@
         <v>0.75</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1"/>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="D7" s="5">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1024,31 +1162,47 @@
         <v>0.85</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="5">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="4"/>
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="4"/>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="4"/>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1059,26 +1213,41 @@
         <v>0.75</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="5">
         <v>0.87</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="4"/>
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1086,10 +1255,14 @@
         <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1100,15 +1273,23 @@
         <v>0.87</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="5">
         <v>0.62</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chapitre 11 et mémoire
</commit_message>
<xml_diff>
--- a/Seconde/2-03.xlsx
+++ b/Seconde/2-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lycée\Seconde\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003A2FE5-54C8-47F3-8945-CA0B5B203CAB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB81DD88-F55B-42CD-A012-F77E03FF4A43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E61A21D0-7BED-4373-9982-F4856F8C3D3D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
   <si>
     <t>Eval Blanche Lewis</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>2.5</t>
+  </si>
+  <si>
+    <t>Note sur 4</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -289,6 +292,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6C7542E-EFA5-4F51-876B-29131A83BB32}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,10 +624,10 @@
     <col min="6" max="6" width="1.6328125" customWidth="1"/>
     <col min="7" max="7" width="24.54296875" customWidth="1"/>
     <col min="8" max="8" width="21.7265625" customWidth="1"/>
-    <col min="9" max="9" width="25.6328125" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -643,8 +649,11 @@
       <c r="H1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I1" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -659,8 +668,11 @@
       <c r="I2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -686,8 +698,11 @@
       <c r="I3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -699,8 +714,11 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -717,11 +735,14 @@
         <v>57</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5">
+      <c r="I5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -742,8 +763,11 @@
       <c r="I6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -763,8 +787,11 @@
       <c r="I7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -779,8 +806,11 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -803,8 +833,11 @@
       <c r="I9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -830,8 +863,11 @@
       <c r="I10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -845,8 +881,11 @@
       <c r="I11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -866,8 +905,11 @@
       <c r="I12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -884,8 +926,11 @@
       <c r="I13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -909,8 +954,11 @@
       <c r="I14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -933,8 +981,11 @@
       <c r="I15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -954,8 +1005,11 @@
       <c r="I16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -981,8 +1035,11 @@
       <c r="I17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1005,8 +1062,11 @@
       <c r="I18">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1017,6 +1077,9 @@
       <c r="H19" s="4"/>
       <c r="I19">
         <v>3.5</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>